<commit_message>
cleaned up input and output
</commit_message>
<xml_diff>
--- a/Max's Budget.xlsx
+++ b/Max's Budget.xlsx
@@ -424,127 +424,127 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Paychecks</t>
+          <t>Bonuses</t>
         </is>
       </c>
       <c r="B1" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Movies</t>
+          <t>Auto Repair/Transportation</t>
         </is>
       </c>
       <c r="D1" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Investments</t>
+          <t>Interest Income</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5005</v>
+        <v>2000</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Music</t>
+          <t>Clothing</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>80</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Returned Purchases</t>
+          <t>Investments</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Streaming Services/Subscriptions</t>
+          <t>Debt &amp; Interest Payments</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>80</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bonuses</t>
+          <t>Paychecks</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>50</v>
+        <v>3000</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Eating Out/Delivery</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>80</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Interest Income</t>
+          <t>Reimbursements</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Eating Out/Delivery</t>
+          <t>Education Expenses</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>80</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Reimbursements</t>
+          <t>Rental Incomes</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>50</v>
+        <v>1000</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Gifts/Donations</t>
+          <t>Electronics/Virtual Products</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>80</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Rental Incomes</t>
+          <t>Returned Purchases</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Health/Medical</t>
+          <t>Fees &amp; Charges</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>10</v>
+        <v>500</v>
       </c>
     </row>
     <row r="8">
@@ -560,37 +560,37 @@
     <row r="9">
       <c r="C9" t="inlineStr">
         <is>
-          <t>Rent</t>
+          <t>Gifts/Donations</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
       <c r="C10" t="inlineStr">
         <is>
-          <t>Auto Repair/Transportation</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11">
       <c r="C11" t="inlineStr">
         <is>
-          <t>Pets</t>
+          <t>Health/Medical</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
       <c r="C12" t="inlineStr">
         <is>
-          <t>Utilities</t>
+          <t>Movies</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -600,11 +600,11 @@
     <row r="13">
       <c r="C13" t="inlineStr">
         <is>
-          <t>Debt &amp; Interest Payments</t>
+          <t>Music</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -614,23 +614,23 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>10</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15">
       <c r="C15" t="inlineStr">
         <is>
-          <t>Clothing</t>
+          <t>Pets</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="C16" t="inlineStr">
         <is>
-          <t>Electronics/Virtual Products</t>
+          <t>Phone</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -640,41 +640,41 @@
     <row r="17">
       <c r="C17" t="inlineStr">
         <is>
-          <t>Education Expenses</t>
+          <t>Rent</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18">
       <c r="C18" t="inlineStr">
         <is>
-          <t>Phone</t>
+          <t>Streaming Services/Subscriptions</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="C19" t="inlineStr">
         <is>
-          <t>Fees &amp; Charges</t>
+          <t>Travel</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>100</v>
+        <v>300</v>
       </c>
     </row>
     <row r="20">
       <c r="C20" t="inlineStr">
         <is>
-          <t>Travel</t>
+          <t>Utilities</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>